<commit_message>
add all ten locations
</commit_message>
<xml_diff>
--- a/magodo.xlsx
+++ b/magodo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oolaonipekun\Desktop\Weather_instrument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A05DA30-1B68-4AF4-8561-C028DBADB46B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01EC6D9-886A-458C-848B-E917BA55374C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{334D9045-CA01-4392-9123-ED4C80381E15}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>